<commit_message>
ref #29 ajuste nos documentos, modificação dos checklists para planilhas
</commit_message>
<xml_diff>
--- a/artefatos_de_processo/VAL/Checklists/RELPREV-022013-VAL-checklist_verificacao_arquitetural.xlsx
+++ b/artefatos_de_processo/VAL/Checklists/RELPREV-022013-VAL-checklist_verificacao_arquitetural.xlsx
@@ -7,19 +7,18 @@
     <workbookView xWindow="480" yWindow="105" windowWidth="12435" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Checklist" sheetId="1" r:id="rId1"/>
+    <sheet name="Deficiências" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_GoBack" localSheetId="0">Plan1!$A$1</definedName>
+    <definedName name="_GoBack" localSheetId="0">Checklist!$A$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Checklist de Verificação Arquitetural</t>
   </si>
@@ -58,6 +57,27 @@
   </si>
   <si>
     <t>Perspectivas</t>
+  </si>
+  <si>
+    <t>Desenvolvedores</t>
+  </si>
+  <si>
+    <t>Arquiteto</t>
+  </si>
+  <si>
+    <t>Dono de Produto</t>
+  </si>
+  <si>
+    <t>Lista de Deficiências Encontradas</t>
+  </si>
+  <si>
+    <t>Item #</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Ação Corretiva</t>
   </si>
 </sst>
 </file>
@@ -94,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -247,11 +267,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -265,6 +309,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -274,27 +321,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -304,7 +351,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -735,56 +791,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="29.25" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="68.25" customHeight="1" thickBot="1">
+    <row r="4" spans="1:5" ht="68.25" customHeight="1" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -792,10 +848,8 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="54.75" customHeight="1" thickBot="1">
+    </row>
+    <row r="5" spans="1:5" ht="54.75" customHeight="1" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -803,10 +857,8 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="48.75" customHeight="1" thickBot="1">
+    </row>
+    <row r="6" spans="1:5" ht="48.75" customHeight="1" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -814,142 +866,116 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="10" t="s">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="9"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="12"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="9"/>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="12"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="17" t="s">
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1">
-      <c r="A13" s="18" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" customHeight="1">
+      <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" spans="1:7" ht="45" customHeight="1">
-      <c r="A14" s="18" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="45" customHeight="1">
+      <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="1:7" ht="45" customHeight="1">
-      <c r="A15" s="18" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="45" customHeight="1">
+      <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="1:7" ht="78.75" customHeight="1">
-      <c r="A17" s="17" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" ht="78.75" customHeight="1">
+      <c r="A17" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" hidden="1" thickBot="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" hidden="1" thickBot="1">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A7:G10"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A7:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:E12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -959,24 +985,185 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:C23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="68.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>